<commit_message>
add param opt for smae t 28
</commit_message>
<xml_diff>
--- a/backtest/bt_report/rs_m_ind/single_run/summary.xlsx
+++ b/backtest/bt_report/rs_m_ind/single_run/summary.xlsx
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="B27" s="7" t="n">
-        <v>0.4363738647635687</v>
+        <v>0.4363738647635688</v>
       </c>
       <c r="C27" s="13" t="n"/>
       <c r="D27" s="13" t="n"/>
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B29" s="7" t="n">
-        <v>0.2533800203278528</v>
+        <v>0.2533800203278527</v>
       </c>
       <c r="C29" s="13" t="n"/>
       <c r="D29" s="13" t="n"/>

</xml_diff>